<commit_message>
fix: avoid using formatRawCellContents() for number cell formatting because it ignores conditional formatting
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.2.103\Root\Download\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952ABBEC-ED56-48FD-BEA5-0559BB59955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2805" yWindow="1980" windowWidth="23355" windowHeight="14145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -60,61 +69,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -148,6 +110,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,24 +442,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>B3+C3</f>
         <v>3</v>
@@ -501,20 +471,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"AAAAA"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"AAAAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: avoid using formatRawCellContents() for number cell formatting because it ignores conditional formatting (#5725)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.2.103\Root\Download\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952ABBEC-ED56-48FD-BEA5-0559BB59955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2805" yWindow="1980" windowWidth="23355" windowHeight="14145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -60,61 +69,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -148,6 +110,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,24 +442,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>B3+C3</f>
         <v>3</v>
@@ -501,20 +471,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"AAAAA"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"AAAAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: avoid using formatRawCellContents() for number cell formatting because it ignores conditional formatting (#5725) (#5757)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.2.103\Root\Download\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952ABBEC-ED56-48FD-BEA5-0559BB59955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2805" yWindow="1980" windowWidth="23355" windowHeight="14145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -60,61 +69,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -148,6 +110,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,24 +442,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>B3+C3</f>
         <v>3</v>
@@ -501,20 +471,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"AAAAA"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"AAAAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: avoid using formatRawCellContents() for number cell formatting because it ignores conditional formatting (#5725) (#5758)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet-flow-integration-tests/src/main/resources/test_sheets/conditional_formatting.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.2.103\Root\Download\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952ABBEC-ED56-48FD-BEA5-0559BB59955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2805" yWindow="1980" windowWidth="23355" windowHeight="14145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -60,61 +69,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -148,6 +110,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,24 +442,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>B3+C3</f>
         <v>3</v>
@@ -501,20 +471,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"AAAAA"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"O"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"AAAAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>